<commit_message>
Promoted source code: 20200324 (E19-026 HCVS hotline service) Promoted Source code 20200319 (I-E19-002 To handle special characters in HA_MingLiu) 20200325 (INT20-0005 Fix report content page display order) 20200331 (E19-030 Revamp of SDIR and VBE) 20200331 (E16-022 SDIR Remark) 20200401 (E19-030-02 Revamp of SDIR and VBE - Phase 2) 20200406 (S20-001 Update covering note)
</commit_message>
<xml_diff>
--- a/EHS2019/ExcelGenerator/Template/eHSM0005-SP_Data_File_Template.xlsx
+++ b/EHS2019/ExcelGenerator/Template/eHSM0005-SP_Data_File_Template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2019\CRE16-022 (SDIR Remark)\Front-end\ExcelGenerator\Template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="19230" windowHeight="6060" tabRatio="679"/>
   </bookViews>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
   <si>
     <t>Sub Report ID</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -341,12 +346,18 @@
   </si>
   <si>
     <t>Provide DHC-related Services</t>
+  </si>
+  <si>
+    <t>CRE16-022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To add a new optional field “Remarks” in the eHS(S) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
@@ -639,6 +650,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -686,7 +700,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -721,7 +735,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1283,9 +1297,8 @@
     <col min="27" max="27" width="26.7109375" style="5" customWidth="1"/>
     <col min="28" max="28" width="26.7109375" style="40" customWidth="1"/>
     <col min="29" max="74" width="22.7109375" style="5" customWidth="1"/>
-    <col min="75" max="85" width="27.7109375" style="5" customWidth="1"/>
-    <col min="86" max="119" width="20.7109375" style="5" customWidth="1"/>
-    <col min="120" max="16384" width="9.140625" style="5"/>
+    <col min="75" max="108" width="20.7109375" style="5" customWidth="1"/>
+    <col min="109" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75">
@@ -1586,7 +1599,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1703,6 +1716,20 @@
         <v>43795</v>
       </c>
     </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="40">
+        <v>7</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="9">
+        <v>43921</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>